<commit_message>
Passeando por todas as paginas
</commit_message>
<xml_diff>
--- a/Produtos.xlsx
+++ b/Produtos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kindle 10a. geração com bateria de longa duração - Cor Preta</t>
+          <t>Fire TV Stick Lite com Controle Remoto Lite por Voz com Alexa (sem controles de TV) | Streaming em Full HD | Modelo 2020</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 399,00</t>
+          <t>R$ 259,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Kindle-10a-gera%C3%A7%C3%A3o-ilumina%C3%A7%C3%A3o-embutida/dp/B07FQK1TS9/ref=zg_bs_electronics_1/142-6465926-6065833?pd_rd_i=B07FQK1TS9&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Novo_FireTVStick_Lite/dp/B07ZZW745X/ref=zg_bs_electronics_1/132-5479222-0411803?pd_rd_i=B07ZZW745X&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -480,17 +480,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fire TV Stick Lite com Controle Remoto Lite por Voz com Alexa (sem controles de TV) | Streaming em Full HD | Modelo 2020</t>
+          <t>Kindle 10a. geração com bateria de longa duração - Cor Preta</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 229,00</t>
+          <t>R$ 399,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Novo_FireTVStick_Lite/dp/B07ZZW745X/ref=zg_bs_electronics_2/142-6465926-6065833?pd_rd_i=B07ZZW745X&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Kindle-10a-gera%C3%A7%C3%A3o-ilumina%C3%A7%C3%A3o-embutida/dp/B07FQK1TS9/ref=zg_bs_electronics_2/132-5479222-0411803?pd_rd_i=B07FQK1TS9&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -512,7 +512,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Novo-Echo-Dot-4%C2%AA-gera%C3%A7%C3%A3o/dp/B084DWCZY6/ref=zg_bs_electronics_3/142-6465926-6065833?pd_rd_i=B084DWCZY6&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Novo-Echo-Dot-4%C2%AA-gera%C3%A7%C3%A3o/dp/B084DWCZY6/ref=zg_bs_electronics_3/132-5479222-0411803?pd_rd_i=B084DWCZY6&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -529,12 +529,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 1.324,00</t>
+          <t>R$ 1.295,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/REDMI-NOTE-TWILIGHT-BLUE-128GB/dp/B09QSC4HN9/ref=zg_bs_electronics_4/142-6465926-6065833?pd_rd_i=B09QSC4HN9&amp;psc=1</t>
+          <t>https://www.amazon.com.br/REDMI-NOTE-TWILIGHT-BLUE-128GB/dp/B09QSC4HN9/ref=zg_bs_electronics_4/132-5479222-0411803?pd_rd_i=B09QSC4HN9&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -546,17 +546,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>iClamper Energia 5 Tomadas - Filtro de Linha + DPS - Preto, Comprimento do cabo de entrada: 1,5 m</t>
+          <t>Echo Dot (3ª Geração): Smart Speaker com Alexa - Cor Preta</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 49,90</t>
+          <t>R$ 349,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Filtro-linha-tomadas-iClamper-Energia/dp/B0763VCVYD/ref=zg_bs_electronics_5/142-6465926-6065833?pd_rd_i=B0763VCVYD&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Echo-Dot-3%C2%AA-Gera%C3%A7%C3%A3o-Cor-Preta/dp/B07PDHSJ1H/ref=zg_bs_electronics_5/132-5479222-0411803?pd_rd_i=B07PDHSJ1H&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -568,17 +568,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Echo Dot (3ª Geração): Smart Speaker com Alexa - Cor Preta</t>
+          <t>iClamper Energia 5 Tomadas - Filtro de Linha + DPS - Preto, Comprimento do cabo de entrada: 1,5 m</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 349,00</t>
+          <t>R$ 49,90</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Echo-Dot-3%C2%AA-Gera%C3%A7%C3%A3o-Cor-Preta/dp/B07PDHSJ1H/ref=zg_bs_electronics_6/142-6465926-6065833?pd_rd_i=B07PDHSJ1H&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Filtro-linha-tomadas-iClamper-Energia/dp/B0763VCVYD/ref=zg_bs_electronics_6/132-5479222-0411803?pd_rd_i=B0763VCVYD&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Kindle-Paperwhite-8GB/dp/B08N3J8GTX/ref=zg_bs_electronics_7/142-6465926-6065833?pd_rd_i=B08N3J8GTX&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Kindle-Paperwhite-8GB/dp/B08N3J8GTX/ref=zg_bs_electronics_7/132-5479222-0411803?pd_rd_i=B08N3J8GTX&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Fire-TV-Stick-Streaming/dp/B08C1K6LB2/ref=zg_bs_electronics_8/142-6465926-6065833?pd_rd_i=B08C1K6LB2&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Fire-TV-Stick-Streaming/dp/B08C1K6LB2/ref=zg_bs_electronics_8/132-5479222-0411803?pd_rd_i=B08C1K6LB2&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -634,17 +634,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Xiaomi Redmi Note 10S 128gb 6gb RAM</t>
+          <t>Pilha Alcalina AA Pequena DURACELL Com 16 Unidades</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 1.464,00</t>
+          <t>R$ 68,90</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Xiaomi-Redmi-Note-10S-128gb/dp/B093FJZYZ5/ref=zg_bs_electronics_9/142-6465926-6065833?pd_rd_i=B093FJZYZ5&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Pilha-Alcalina-Pequena-Duracell-3020720/dp/B0778VZYVV/ref=zg_bs_electronics_9/132-5479222-0411803?pd_rd_i=B0778VZYVV&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -656,17 +656,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Apple iPad 9 Geração 10.2" Wi-Fi 64gb Cinza Espacial MK2K3LL/A</t>
+          <t>Xiaomi Redmi Note 10S 128gb 6gb RAM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 3.881,00</t>
+          <t>R$ 1.464,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Apple-Gera%C3%A7%C3%A3o-Wi-Fi-Espacial-MK2K3LL/dp/B09G9FPHY6/ref=zg_bs_electronics_10/142-6465926-6065833?pd_rd_i=B09G9FPHY6&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Xiaomi-Redmi-Note-10S-128gb/dp/B093FJZYZ5/ref=zg_bs_electronics_10/132-5479222-0411803?pd_rd_i=B093FJZYZ5&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -678,17 +678,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Pilha Alcalina AA Pequena DURACELL Com 16 Unidades</t>
+          <t>Kindle 10a. geração com bateria de longa duração - Cor Branca</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 68,90</t>
+          <t>R$ 399,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Pilha-Alcalina-Pequena-Duracell-3020720/dp/B0778VZYVV/ref=zg_bs_electronics_11/142-6465926-6065833?pd_rd_i=B0778VZYVV&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Kindle-10a-gera%C3%A7%C3%A3o-ilumina%C3%A7%C3%A3o-embutida/dp/B07FPX33X5/ref=zg_bs_electronics_11/132-5479222-0411803?pd_rd_i=B07FPX33X5&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -700,17 +700,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kindle 10a. geração com bateria de longa duração - Cor Branca</t>
+          <t>Redmi Note 10S Starlight Purple 6GB RAM 128GB ROM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 399,00</t>
+          <t>R$ 1.479,97</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Kindle-10a-gera%C3%A7%C3%A3o-ilumina%C3%A7%C3%A3o-embutida/dp/B07FPX33X5/ref=zg_bs_electronics_12/142-6465926-6065833?pd_rd_i=B07FPX33X5&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Redmi-Note-Starlight-Purple-128GB/dp/B09DD8J1RS/ref=zg_bs_electronics_12/132-5479222-0411803?pd_rd_i=B09DD8J1RS&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -722,17 +722,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>IPAD WIFI 64GB SILVER 9° GERAÇÃO MK2L3LL/A</t>
+          <t>Pilha Alcalina AAA Palito DURACELL com 16 unidades</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>R$ 3.981,00</t>
+          <t>R$ 68,90</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/IPAD-WIFI-SILVER-GERA%C3%87%C3%83O-MK2L3LL/dp/B09G9CJM1Z/ref=zg_bs_electronics_13/142-6465926-6065833?pd_rd_i=B09G9CJM1Z&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Pilha-Alcalina-Palito-Duracell-3020719/dp/B078GSWP44/ref=zg_bs_electronics_13/132-5479222-0411803?pd_rd_i=B078GSWP44&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -744,17 +744,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Xiaomi Redmi Note 10S 128gb 6gb Azul</t>
+          <t>Filtro De Linha 5 Tomadas Preto Multilaser - WI297</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>R$ 1.513,90</t>
+          <t>R$ 22,99</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Xiaomi-Redmi-Note-10S-128gb/dp/B0979PF8F4/ref=zg_bs_electronics_14/142-6465926-6065833?pd_rd_i=B0979PF8F4&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Filtro-Linha-Tomadas-Multilaser-Preto/dp/B075JSQ8CK/ref=zg_bs_electronics_14/132-5479222-0411803?pd_rd_i=B075JSQ8CK&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -766,17 +766,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Filtro De Linha 5 Tomadas Preto Multilaser - WI297</t>
+          <t>Xiaomi Redmi Note 10S 128gb 6gb Azul</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 22,99</t>
+          <t>R$ 1.486,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Filtro-Linha-Tomadas-Multilaser-Preto/dp/B075JSQ8CK/ref=zg_bs_electronics_15/142-6465926-6065833?pd_rd_i=B075JSQ8CK&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Xiaomi-Redmi-Note-10S-128gb/dp/B0979PF8F4/ref=zg_bs_electronics_15/132-5479222-0411803?pd_rd_i=B0979PF8F4&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -788,17 +788,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Carregador de Pilhas Recarregáveis AA e AAA DURACELL Com 4 Pilhas AA</t>
+          <t>FILTRO DE LINHA C/ 5 TOMADAS EPE 205 PT 4824201</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 180,90</t>
+          <t>R$ 24,90</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Carregador-Pilhas-com-pilhas-Duracell/dp/B07X4JG2G4/ref=zg_bs_electronics_16/142-6465926-6065833?pd_rd_i=B07X4JG2G4&amp;psc=1</t>
+          <t>https://www.amazon.com.br/FILTRO-LINHA-TOMADAS-EPE-4824201/dp/B08BKZCHGM/ref=zg_bs_electronics_16/132-5479222-0411803?pd_rd_i=B08BKZCHGM&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -810,17 +810,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Redmi Note 10S Starlight Purple 6GB RAM 128GB ROM</t>
+          <t>Protetor Eletronico Intelbras com 8 tomadas EPE 1008+ Branco</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 1.529,00</t>
+          <t>R$ 36,90</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Redmi-Note-Starlight-Purple-128GB/dp/B09DD8J1RS/ref=zg_bs_electronics_17/142-6465926-6065833?pd_rd_i=B09DD8J1RS&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Protetor-Eletr%C3%B4nico-Intelbras-EPE-1008/dp/B07DGFSMZP/ref=zg_bs_electronics_17/132-5479222-0411803?pd_rd_i=B07DGFSMZP&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -832,17 +832,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PHILCO Fast Smart TV 32" PTV32G70RCH Roku Tv Led</t>
+          <t>Carregador de Pilhas Recarregáveis AA e AAA DURACELL Com 4 Pilhas AA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>R$ 1.199,00</t>
+          <t>R$ 180,90</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/PHILCO-Fast-Smart-PTV32G70RCH-Roku/dp/B09PNQZ8VH/ref=zg_bs_electronics_18/142-6465926-6065833?pd_rd_i=B09PNQZ8VH&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Carregador-Pilhas-com-pilhas-Duracell/dp/B07X4JG2G4/ref=zg_bs_electronics_18/132-5479222-0411803?pd_rd_i=B07X4JG2G4&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -854,17 +854,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>FILTRO DE LINHA C/ 5 TOMADAS EPE 205 PT 4824201</t>
+          <t>Echo Dot (4ª Geração): Smart Speaker com Alexa - Cor Azul</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>R$ 24,90</t>
+          <t>R$ 399,00</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/FILTRO-LINHA-TOMADAS-EPE-4824201/dp/B08BKZCHGM/ref=zg_bs_electronics_19/142-6465926-6065833?pd_rd_i=B08BKZCHGM&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-Gera%C3%A7%C3%A3o-Speaker/dp/B084KV8YRR/ref=zg_bs_electronics_19/132-5479222-0411803?pd_rd_i=B084KV8YRR&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -876,17 +876,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pilha Alcalina AAA Palito DURACELL com 16 unidades</t>
+          <t>Echo Dot (4ª Geração): Smart Speaker com Alexa - Cor Branca</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>R$ 68,90</t>
+          <t>R$ 399,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Pilha-Alcalina-Palito-Duracell-3020719/dp/B078GSWP44/ref=zg_bs_electronics_20/142-6465926-6065833?pd_rd_i=B078GSWP44&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-Gera%C3%A7%C3%A3o-Speaker/dp/B084KQBYYM/ref=zg_bs_electronics_20/132-5479222-0411803?pd_rd_i=B084KQBYYM&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -898,17 +898,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Echo Dot (4ª Geração): Smart Speaker com Alexa - Cor Branca</t>
+          <t>PHILCO Fast Smart TV 32" PTV32G70RCH Roku Tv Led</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>R$ 399,00</t>
+          <t>R$ 1.199,00</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-Gera%C3%A7%C3%A3o-Speaker/dp/B084KQBYYM/ref=zg_bs_electronics_21/142-6465926-6065833?pd_rd_i=B084KQBYYM&amp;psc=1</t>
+          <t>https://www.amazon.com.br/PHILCO-Fast-Smart-PTV32G70RCH-Roku/dp/B09PNQZ8VH/ref=zg_bs_electronics_21/132-5479222-0411803?pd_rd_i=B09PNQZ8VH&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -920,17 +920,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Protetor Eletronico Intelbras com 8 tomadas EPE 1008+ Branco</t>
+          <t>Apple iPad 9 Geração 10.2" Wi-Fi 64gb Cinza Espacial MK2K3LL/A</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>R$ 36,90</t>
+          <t>R$ --------</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Protetor-Eletr%C3%B4nico-Intelbras-EPE-1008/dp/B07DGFSMZP/ref=zg_bs_electronics_22/142-6465926-6065833?pd_rd_i=B07DGFSMZP&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Apple-Gera%C3%A7%C3%A3o-Wi-Fi-Espacial-MK2K3LL/dp/B09G9FPHY6/ref=zg_bs_electronics_22/132-5479222-0411803?pd_rd_i=B09G9FPHY6&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -942,17 +942,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kit Pilhas Alcalinas com 2X AAA Palito, Elgin, Baterias</t>
+          <t>Roku Express - Streaming player Full HD. Transforma sua TV em Smart TV. Com controle remoto e cabo HDMI incluídos.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>R$ 4,41</t>
+          <t>R$ 259,90</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Pilhas-Alcalinas-Palito-Elgin-Baterias/dp/B0754C87VL/ref=zg_bs_electronics_23/142-6465926-6065833?pd_rd_i=B0754C87VL&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Roku-Express-Streaming-Transforma-inclu%C3%ADdos/dp/B09KNTBKMP/ref=zg_bs_electronics_23/132-5479222-0411803?pd_rd_i=B09KNTBKMP&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -964,17 +964,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pilha Recarregável AAA Blister Com 4 Pilhas, Elgin, Baterias, 1000mAh</t>
+          <t>Smart TV LED 32" HD LG 32LM621CBSB.A, 3 HDMI, 2 USB, Bluetooth, Wi-Fi, Active HDR, ThinQ AI</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>R$ 28,90</t>
+          <t>R$ 1.374,51</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Recarreg%C3%A1vel-AAA-1000Mah-Blister-Elgin-Baterias/dp/B0754KMGFN/ref=zg_bs_electronics_24/142-6465926-6065833?pd_rd_i=B0754KMGFN&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Smart-LG-Bluetooth-Active-32LM621CBSB/dp/B07WBV8CCJ/ref=zg_bs_electronics_24/132-5479222-0411803?pd_rd_i=B07WBV8CCJ&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -986,17 +986,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Roku Express - Streaming player Full HD. Transforma sua TV em Smart TV. Com controle remoto e cabo HDMI incluídos.</t>
+          <t>Fujifilm 705061900 - Filme Instax Mini, 6 x 10 Folhas de Fotos</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>R$ 259,90</t>
+          <t>R$ 198,95</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Roku-Express-Streaming-Transforma-inclu%C3%ADdos/dp/B09KNTBKMP/ref=zg_bs_electronics_25/142-6465926-6065833?pd_rd_i=B09KNTBKMP&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Filme-Instax-Fotos-Fujifilm-Filmes/dp/B0778LV53L/ref=zg_bs_electronics_25/132-5479222-0411803?pd_rd_i=B0778LV53L&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1008,17 +1008,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Adaptador de energia</t>
+          <t>Pilha Recarregável AAA Blister Com 4 Pilhas, Elgin, Baterias, 1000mAh</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>R$ 99,00</t>
+          <t>R$ 27,92</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Amazon-53-024641-Adaptador-de-energia/dp/B086ZK1PP5/ref=zg_bs_electronics_26/142-6465926-6065833?pd_rd_i=B086ZK1PP5&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Recarreg%C3%A1vel-AAA-1000Mah-Blister-Elgin-Baterias/dp/B0754KMGFN/ref=zg_bs_electronics_26/132-5479222-0411803?pd_rd_i=B0754KMGFN&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1030,17 +1030,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Câmera de Monitoramento 360º, Wi-Fi Full HD, Tapo C200, TP-Link</t>
+          <t>Kit Pilhas Alcalinas com 2X AAA Palito, Elgin, Baterias</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>R$ 279,00</t>
+          <t>R$ 4,41</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/C%C3%A2mera-Monitoramento-Tapo-C200-TP-Link/dp/B07XLML2YS/ref=zg_bs_electronics_27/142-6465926-6065833?pd_rd_i=B09SH9XP5C&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Pilhas-Alcalinas-Palito-Elgin-Baterias/dp/B0754C87VL/ref=zg_bs_electronics_27/132-5479222-0411803?pd_rd_i=B0754C87VL&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1052,17 +1052,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Novo Kindle Paperwhite Signature Edition (32 GB): tela de 6,8", carregamento sem fio e luz frontal adaptável</t>
+          <t>Echo Dot (4ª geração): Smart Speaker com Relógio e Alexa - Cor Branca</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>R$ 849,00</t>
+          <t>R$ 499,00</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Kindle-Paperwhite-32GB/dp/B08N2ZL7PS/ref=zg_bs_electronics_28/142-6465926-6065833?pd_rd_i=B08N2ZL7PS&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Novo-Echo-Dot-com-rel%C3%B3gio/dp/B084J4WP6J/ref=zg_bs_electronics_28/132-5479222-0411803?pd_rd_i=B084J4WP6J&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1074,17 +1074,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Echo Dot (4ª Geração): Smart Speaker com Alexa - Cor Azul</t>
+          <t>Carregador de Pilhas Multilaser AA/AAA + 4 Pilhas AA 2500Mah - CB054, turquoise</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>R$ 399,00</t>
+          <t>R$ 72,90</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-Gera%C3%A7%C3%A3o-Speaker/dp/B084KV8YRR/ref=zg_bs_electronics_29/142-6465926-6065833?pd_rd_i=B084KV8YRR&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Carregador-Pilhas-AAA-2500-mAh/dp/B0754CL6S7/ref=zg_bs_electronics_29/132-5479222-0411803?pd_rd_i=B0754CL6S7&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Kit-Pilhas-Alcalinas-Elgin-Baterias/dp/B0754KGXV2/ref=zg_bs_electronics_30/142-6465926-6065833?pd_rd_i=B0754KGXV2&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Kit-Pilhas-Alcalinas-Elgin-Baterias/dp/B0754KGXV2/ref=zg_bs_electronics_30/132-5479222-0411803?pd_rd_i=B0754KGXV2&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1118,17 +1118,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Smart TV LED 32" HD LG 32LM621CBSB.A, 3 HDMI, 2 USB, Bluetooth, Wi-Fi, Active HDR, ThinQ AI</t>
+          <t>Adaptador de energia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>R$ 1.374,51</t>
+          <t>R$ 99,00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Smart-LG-Bluetooth-Active-32LM621CBSB/dp/B07WBV8CCJ/ref=zg_bs_electronics_31/142-6465926-6065833?pd_rd_i=B07WBV8CCJ&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Amazon-53-024641-Adaptador-de-energia/dp/B086ZK1PP5/ref=zg_bs_electronics_31/132-5479222-0411803?pd_rd_i=B086ZK1PP5&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1140,17 +1140,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Echo Dot (4ª geração): Smart Speaker com Relógio e Alexa - Cor Branca</t>
+          <t>Xiaomi Smartphone Poco F3 256GB 8GB RAM Night Black - Preto</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>R$ 499,00</t>
+          <t>R$ 2.261,60</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Novo-Echo-Dot-com-rel%C3%B3gio/dp/B084J4WP6J/ref=zg_bs_electronics_32/142-6465926-6065833?pd_rd_i=B084J4WP6J&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Smartphone-Poco-256gb-8gb-RAM/dp/B091BSTQM8/ref=zg_bs_electronics_32/132-5479222-0411803?pd_rd_i=B091BSTQM8&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1162,17 +1162,17 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Carregador de Pilhas Multilaser AA/AAA + 4 Pilhas AA 2500Mah - CB054, turquoise</t>
+          <t>Câmera de Monitoramento 360º, Wi-Fi Full HD, Tapo C200, TP-Link</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>R$ 72,90</t>
+          <t>R$ 279,90</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Carregador-Pilhas-AAA-2500-mAh/dp/B0754CL6S7/ref=zg_bs_electronics_33/142-6465926-6065833?pd_rd_i=B0754CL6S7&amp;psc=1</t>
+          <t>https://www.amazon.com.br/C%C3%A2mera-Monitoramento-Tapo-C200-TP-Link/dp/B07XLML2YS/ref=zg_bs_electronics_33/132-5479222-0411803?pd_rd_i=B09SH9XP5C&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1184,17 +1184,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Fujifilm 705061900 - Filme Instax Mini, 6 x 10 Folhas de Fotos</t>
+          <t>Novo Kindle Paperwhite Signature Edition (32 GB): tela de 6,8", carregamento sem fio e luz frontal adaptável</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>R$ 189,00</t>
+          <t>R$ 849,00</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Filme-Instax-Fotos-Fujifilm-Filmes/dp/B0778LV53L/ref=zg_bs_electronics_34/142-6465926-6065833?pd_rd_i=B0778LV53L&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Kindle-Paperwhite-32GB/dp/B08N2ZL7PS/ref=zg_bs_electronics_34/132-5479222-0411803?pd_rd_i=B08N2ZL7PS&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1206,17 +1206,17 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Smartphone Poco X3 PRO 256gb 8gb RAM – Phantom Black - Preto</t>
+          <t>Echo (4ª Geração): Com som premium, hub de casa inteligente e Alexa - Cor Preta</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>R$ 2.299,90</t>
+          <t>R$ 699,00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Smartphone-Poco-PRO-256gb-8gb/dp/B0919PLV7S/ref=zg_bs_electronics_35/142-6465926-6065833?pd_rd_i=B0919PLV7S&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Novo-Echo-4%C2%AA-gera%C3%A7%C3%A3o/dp/B085FXDTTX/ref=zg_bs_electronics_35/132-5479222-0411803?pd_rd_i=B085FXDTTX&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1233,12 +1233,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>R$ 1.555,00</t>
+          <t>R$ 1.469,90</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/SMARTPHONE-XIAOMI-REDMI-NOTE-128GB/dp/B098FKC3VX/ref=zg_bs_electronics_36/142-6465926-6065833?pd_rd_i=B098FKC3VX&amp;psc=1</t>
+          <t>https://www.amazon.com.br/SMARTPHONE-XIAOMI-REDMI-NOTE-128GB/dp/B098FKC3VX/ref=zg_bs_electronics_36/132-5479222-0411803?pd_rd_i=B098FKC3VX&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1250,17 +1250,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Echo (4ª Geração): Com som premium, hub de casa inteligente e Alexa - Cor Preta</t>
+          <t>Google Chromecast Hdmi 3 Geração - Preto 1371</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>R$ 699,00</t>
+          <t>R$ 209,99</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Novo-Echo-4%C2%AA-gera%C3%A7%C3%A3o/dp/B085FXDTTX/ref=zg_bs_electronics_37/142-6465926-6065833?pd_rd_i=B085FXDTTX&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Google-Chromecast-Hdmi-Gera%C3%A7%C3%A3o-Preto/dp/B07NQB6YXD/ref=zg_bs_electronics_37/132-5479222-0411803?pd_rd_i=B07NQB6YXD&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1272,17 +1272,17 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>GALAXY TAB A7 LITE WIFI 8.7 32GB</t>
+          <t>Multiplicador 4 Tomadas Bivolt + 2 USB 2.4A - PowerCube USB ELG - PWC-R4U, Azul e Branco</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>R$ 899,00</t>
+          <t>R$ 80,42</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/GALAXY-TAB-LITE-WIFI-32GB/dp/B09G897XCY/ref=zg_bs_electronics_38/142-6465926-6065833?pd_rd_i=B09G897XCY&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Multiplicador-Tomadas-Bivolt-Elg-PWC-R4U/dp/B077719JMJ/ref=zg_bs_electronics_38/132-5479222-0411803?pd_rd_i=B08FTYKVJ3&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1294,17 +1294,17 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Xiaomi Smartphone Poco F3 256GB 8GB RAM Night Black - Preto</t>
+          <t>IPAD WIFI 64GB SILVER 9° GERAÇÃO MK2L3LL/A</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>R$ 2.279,88</t>
+          <t>R$ --------</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Smartphone-Poco-256gb-8gb-RAM/dp/B091BSTQM8/ref=zg_bs_electronics_39/142-6465926-6065833?pd_rd_i=B091BSTQM8&amp;psc=1</t>
+          <t>https://www.amazon.com.br/IPAD-WIFI-SILVER-GERA%C3%87%C3%83O-MK2L3LL/dp/B09G9CJM1Z/ref=zg_bs_electronics_39/132-5479222-0411803?pd_rd_i=B09G9CJM1Z&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1316,17 +1316,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Echo Dot (4ª geração): Smart Speaker com Relógio e Alexa - Cor Azul</t>
+          <t>Smartphone Poco X3 PRO 256gb 8gb RAM – Phantom Black - Preto</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>R$ 499,00</t>
+          <t>R$ 2.059,90</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-gera%C3%A7%C3%A3o-Speaker/dp/B085M5P9LF/ref=zg_bs_electronics_40/142-6465926-6065833?pd_rd_i=B085M5P9LF&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Smartphone-Poco-PRO-256gb-8gb/dp/B0919PLV7S/ref=zg_bs_electronics_40/132-5479222-0411803?pd_rd_i=B0919PLV7S&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1338,17 +1338,17 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Capa de tecido para Kindle 10ª Geração – Cor Preta (não compatível com o Kindle 8ª Geração)</t>
+          <t>Echo Dot (4ª geração): Smart Speaker com Relógio e Alexa - Cor Azul</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>R$ 89,00</t>
+          <t>R$ 499,00</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Capa-tecido-para-novo-Kindle/dp/B07K8J59VP/ref=zg_bs_electronics_41/142-6465926-6065833?pd_rd_i=B07K8J59VP&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Echo-Dot-4%C2%AA-gera%C3%A7%C3%A3o-Speaker/dp/B085M5P9LF/ref=zg_bs_electronics_41/132-5479222-0411803?pd_rd_i=B085M5P9LF&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1360,17 +1360,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Filtro De Linha 5 Tomadas Branco Multilaser - WI300</t>
+          <t>GALAXY TAB A7 LITE WIFI 8.7 32GB</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>R$ 27,99</t>
+          <t>R$ 899,00</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Filtro-Linha-Tomadas-Multilaser-Branco/dp/B075JSGY4K/ref=zg_bs_electronics_42/142-6465926-6065833?pd_rd_i=B075JSGY4K&amp;psc=1</t>
+          <t>https://www.amazon.com.br/GALAXY-TAB-LITE-WIFI-32GB/dp/B09G897XCY/ref=zg_bs_electronics_42/132-5479222-0411803?pd_rd_i=B09G897XCY&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1382,17 +1382,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 (128 GB) Preto</t>
+          <t>Capa de tecido para Kindle 10ª Geração – Cor Preta (não compatível com o Kindle 8ª Geração)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>R$ 4.099,99</t>
+          <t>R$ 89,00</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Apple-MHDH3BR-A-iPhone-11-128-GB/dp/B08N5G4CM2/ref=zg_bs_electronics_43/142-6465926-6065833?pd_rd_i=B08N5G4CM2&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Capa-tecido-para-novo-Kindle/dp/B07K8J59VP/ref=zg_bs_electronics_43/132-5479222-0411803?pd_rd_i=B07K8J59VP&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1404,17 +1404,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Multiplicador 4 Tomadas Bivolt + 2 USB 2.4A - PowerCube USB ELG - PWC-R4U, Azul e Branco</t>
+          <t>Luz e Iluminador Ring Light 6 Polegadas 36 Led Usb Led Misto Mesa</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>R$ 80,42</t>
+          <t>R$ 34,20</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Multiplicador-Tomadas-Bivolt-Elg-PWC-R4U/dp/B077719JMJ/ref=zg_bs_electronics_44/142-6465926-6065833?pd_rd_i=B08FTYKVJ3&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Iluminador-Ring-Light-Polegadas-Misto/dp/B07TSFLCZR/ref=zg_bs_electronics_44/132-5479222-0411803?pd_rd_i=B07TSFLCZR&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1426,17 +1426,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Luz e Iluminador Ring Light 6 Polegadas 36 Led Usb Led Misto Mesa</t>
+          <t>Xiaomi Smartphone Poco X3 PRO 256GB 8GB RAM Frost Blue - Azul</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>R$ 34,20</t>
+          <t>R$ 2.059,90</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Iluminador-Ring-Light-Polegadas-Misto/dp/B07TSFLCZR/ref=zg_bs_electronics_45/142-6465926-6065833?pd_rd_i=B07TSFLCZR&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Smartphone-Poco-PRO-256gb-8gb/dp/B0919N55XG/ref=zg_bs_electronics_45/132-5479222-0411803?pd_rd_i=B0919N55XG&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1448,17 +1448,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Xiaomi Redmi 10 Prime 6Gb 128Gb - Phantom Black</t>
+          <t>Filtro De Linha 5 Tomadas Branco Multilaser - WI300</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>R$ 1.464,00</t>
+          <t>R$ 27,99</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Xiaomi-Redmi-10-Prime-128Gb/dp/B09CV13RWF/ref=zg_bs_electronics_46/142-6465926-6065833?pd_rd_i=B09CV13RWF&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Filtro-Linha-Tomadas-Multilaser-Branco/dp/B075JSGY4K/ref=zg_bs_electronics_46/132-5479222-0411803?pd_rd_i=B075JSGY4K&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1470,17 +1470,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Apple iPhone 11 (128 GB) Branco</t>
+          <t>Apple iPhone 11 (128 GB) Preto</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>R$ 4.099,99</t>
+          <t>R$ 4.184,07</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/iPhone-Branco-com-Tela-C%C3%83%C2%A2mera/dp/B08NXK32ZX/ref=zg_bs_electronics_47/142-6465926-6065833?pd_rd_i=B08NXK32ZX&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Apple-MHDH3BR-A-iPhone-11-128-GB/dp/B08N5G4CM2/ref=zg_bs_electronics_47/132-5479222-0411803?pd_rd_i=B08N5G4CM2&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Capa-Kindle-Paperwhite-Azul/dp/B08VZCBWN8/ref=zg_bs_electronics_48/142-6465926-6065833?pd_rd_i=B08VZCBWN8&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Capa-Kindle-Paperwhite-Azul/dp/B08VZCBWN8/ref=zg_bs_electronics_48/132-5479222-0411803?pd_rd_i=B08VZCBWN8&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1519,12 +1519,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>R$ 1.749,00</t>
+          <t>R$ 1.690,05</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Android-LED-TCL-S615-FULL/dp/B097Q1RBKG/ref=zg_bs_electronics_49/142-6465926-6065833?pd_rd_i=B097Q1RBKG&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Android-LED-TCL-S615-FULL/dp/B097Q1RBKG/ref=zg_bs_electronics_49/132-5479222-0411803?pd_rd_i=B097Q1RBKG&amp;psc=1</t>
         </is>
       </c>
     </row>
@@ -1536,17 +1536,1117 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Xiaomi Smartphone Poco X3 PRO 256GB 8GB RAM Frost Blue - Azul</t>
+          <t>Xiaomi Redmi 10 Prime 6Gb 128Gb - Phantom Black</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>R$ 2.145,00</t>
+          <t>R$ 1.399,00</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://www.amazon.com.br/Smartphone-Poco-PRO-256gb-8gb/dp/B0919N55XG/ref=zg_bs_electronics_50/142-6465926-6065833?pd_rd_i=B0919N55XG&amp;psc=1</t>
+          <t>https://www.amazon.com.br/Xiaomi-Redmi-10-Prime-128Gb/dp/B09CV13RWF/ref=zg_bs_electronics_50/132-5479222-0411803?pd_rd_i=B09CV13RWF&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>#51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Smartphone Poco X3 PRO 128gb 6gb RAM – Phantom Black - Preto</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>R$ 1.929,00</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Poco-PRO-128gb-6gb/dp/B0919N2P7J/ref=zg_bs_electronics_1/132-5479222-0411803?pd_rd_i=B0919N2P7J&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>#52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Tablet Multilaser M7 Wi-Fi 1+32GB Quad Core Android 11 Preto - NB355</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>R$ 299,00</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Tablet-Multilaser-Wi-Fi-Android-Preto/dp/B097FC1VGX/ref=zg_bs_electronics_2/132-5479222-0411803?pd_rd_i=B097FC1VGX&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>#53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Pilha Recarregável AA Pequena DURACELL Com 4 Unidades</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>R$ 93,88</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Duracell-Recarreg%C3%A1vel-Longa-Vida-Pacote/dp/B00007ISWA/ref=zg_bs_electronics_3/132-5479222-0411803?pd_rd_i=B00007ISWA&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>#54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Smartphone Xiaomi Redmi 9i Sport 64gb / 4gb Ram Tela 6.53 - Carbon Black</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>R$ 914,76</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-Redmi-Sport-64gb/dp/B09HSKYMB3/ref=zg_bs_electronics_4/132-5479222-0411803?pd_rd_i=B09HSKYMB3&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>#55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Celular Xiaomi Poco X3 GT Preto 8/256 Versão Global</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>R$ 2.018,00</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Celular-Xiaomi-Poco-X3-GT/dp/B09B7PM9DF/ref=zg_bs_electronics_5/132-5479222-0411803?pd_rd_i=B09B7PM9DF&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>#56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Tablet Samsung Tab S6 Lite, Wi-Fi, 4G, Câmera 8MP Frontal 5MP, 64GB, Android 10.0, Octa-Core, Tela 10.4", Cinza</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>R$ 2.399,00</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Tablet-Samsung-Android-Octa-Core-Frontal/dp/B00S5C679S/ref=zg_bs_electronics_6/132-5479222-0411803?pd_rd_i=B00S5C679S&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>#57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Apple iPhone 11 (128 GB) Branco</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>R$ 4.184,07</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/iPhone-Branco-com-Tela-C%C3%83%C2%A2mera/dp/B08NXK32ZX/ref=zg_bs_electronics_7/132-5479222-0411803?pd_rd_i=B08NXK32ZX&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>#58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>POCO F3 Artic White 8GB RAM 256GB ROM</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>R$ 2.259,00</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/POCO-F3-Artic-White-256GB/dp/B091C9KNBL/ref=zg_bs_electronics_8/132-5479222-0411803?pd_rd_i=B091C9KNBL&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>#59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Media Receiver Pioneer Mvh-S218Bt</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>R$ 379,90</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/MP3-Player-Pioneer-175630-CD/dp/B07K3Z4912/ref=zg_bs_electronics_9/132-5479222-0411803?pd_rd_i=B07K3Z4912&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>#60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Bateria 9V DURACELL com 1 unidade</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>R$ 17,25</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Bateria-Alcalina-Duracell-1003640-Cinza/dp/B00163G2DO/ref=zg_bs_electronics_10/132-5479222-0411803?pd_rd_i=B00163G2DO&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>#61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Novo Echo Show 5 (2ª Geração, versão 2021): Smart Display de 5" com Alexa e câmera de 2 MP - Cor Preta</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>R$ 599,00</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Echo-Show-5-segunda-gera%C3%A7%C3%A3o-preto/dp/B08KGWJDRZ/ref=zg_bs_electronics_11/132-5479222-0411803?pd_rd_i=B08KGWJDRZ&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>#62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>BATERIA DE LITHIUM 3V COM 1 CR2032</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>R$ 11,50</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/BATERIA-LITHIUM-3V-COM-CR2032/dp/B0081UCM48/ref=zg_bs_electronics_12/132-5479222-0411803?pd_rd_i=B0081UCM48&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>#63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 11 Graphite Gray 6GB Ram 128GB Rom</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>R$ 1.529,90</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Xiaomi-Redmi-Note-11-Graphite/dp/B09QSB4N2C/ref=zg_bs_electronics_13/132-5479222-0411803?pd_rd_i=B09QSB4N2C&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>#64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Smart TV LED 24" Monitor LG 24TL520S, Wi-Fi, WebOS 3.5, DTV Machine Ready</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>R$ 1.079,00</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smart-Monitor-LG-Machine-24TL520S/dp/B07SSCKJJ3/ref=zg_bs_electronics_14/132-5479222-0411803?pd_rd_i=B07SSCKJJ3&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>#65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Pilha Recarregável Ni-MH AAA-900mAh blister com 4 pilhas, Elgin, Baterias, 82169</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>R$ 24,30</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Recarreg%C3%A1vel-AAA-900Mah-Blister-Elgin-Baterias/dp/B0755P2K3M/ref=zg_bs_electronics_15/132-5479222-0411803?pd_rd_i=B0755P2K3M&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>#66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Pilhas Recarregáveis AA Multilaser 2500Mah Com 4 Unidades - CB052, Multicor</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>R$ 45,00</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Recarreg%C3%A1veis-Unidades-Multilaser-CB052-Multicor/dp/B0752GSS56/ref=zg_bs_electronics_16/132-5479222-0411803?pd_rd_i=B0752GSS56&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>#67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Pilha Recarregável Ni-Mh Aa-2500Mah Blister Com 4 Pilhas, Elgin, Baterias</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>R$ 49,90</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Recarreg%C3%A1vel-AA-2500Mah-Blister-Elgin-Baterias/dp/B0755P9SCV/ref=zg_bs_electronics_17/132-5479222-0411803?pd_rd_i=B0755P9SCV&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>#68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>intelbras Vídeo Porteiro com Monofone IVR 1010 Preto, Preto/Branco</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>R$ 457,30</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Porteiro-Monofone-IVR-1010-Intelbras/dp/B079X57PCC/ref=zg_bs_electronics_18/132-5479222-0411803?pd_rd_i=B079X57PCC&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>#69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>PILHA COMUM AA C/4 UM-3SHS</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>R$ 5,99</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Panasonic-UM-3SHS-PILHA-COMUM-AA/dp/B075XFDPL2/ref=zg_bs_electronics_19/132-5479222-0411803?pd_rd_i=B075XFDPL2&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>#70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Tira de Bateria de Lithium Botão, Panasonic, CR2032-1BT</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>R$ 24,69</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Bateria-Lithium-Panasonic-CR2032-1BT-pacote/dp/B076HB92XB/ref=zg_bs_electronics_20/132-5479222-0411803?pd_rd_i=B076HB92XB&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>#71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Xiaomi Smartphone Redmi 9A 32 GB, 2 GB RAM, 6.53 LCD, Sky Blue - Azul</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>R$ 799,00</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-Redmi-9A-32GB/dp/B08CH6X6M5/ref=zg_bs_electronics_21/132-5479222-0411803?pd_rd_i=B08CH6X6M5&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>#72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Receptor De TV Via Internet Full Hd Elsys ETRI01 Smarty, Preto</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>R$ 277,11</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/RECEPTOR-INTERNET-ETRI01-SMARTY-Elsys/dp/B07QZ4GJ2W/ref=zg_bs_electronics_22/132-5479222-0411803?pd_rd_i=B07QZ4GJ2W&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>#73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>PILHA COMUM AAA COM 4 R03UAL/4B400</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>R$ 5,99</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/PILHA-COMUM-AAA-R03UAL-4B400/dp/B075X3H9JZ/ref=zg_bs_electronics_23/132-5479222-0411803?pd_rd_i=B075X3H9JZ&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>#74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Celular Xiaomi Redmi 10 Prime 6Gb 128Gb - Astral White</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>R$ 1.389,00</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Celular-Xiaomi-Redmi-10-Prime/dp/B09CTZ1Z75/ref=zg_bs_electronics_24/132-5479222-0411803?pd_rd_i=B09CTZ1Z75&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>#75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Android TV LED 32” TCL S615 HD HDR</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>R$ 1.299,00</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Android-LED-TCL-S615-HDR/dp/B097Q5MNFV/ref=zg_bs_electronics_25/132-5479222-0411803?pd_rd_i=B097Q5MNFV&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>#76</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Echo Studio - Smart Speaker com áudio de alta fidelidade e Alexa</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>R$ 1.699,00</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Echo-Studio-Smart-Speaker/dp/B07NQBGRKY/ref=zg_bs_electronics_26/132-5479222-0411803?pd_rd_i=B07NQBGRKY&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>#77</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Smartphone Xiaomi Poco X3 GT 5G 8gb 128gb Stargaze Black - Preto</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>R$ 1.788,39</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-128gb-Stargaze-Black/dp/B099QR5XVW/ref=zg_bs_electronics_27/132-5479222-0411803?pd_rd_i=B099QR5XVW&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>#78</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Pilha, Rayovac, Alcalina 208013, Azul, Aa, Pequena, Pacote de 4</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>R$ 10,99</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Pilha-Rayovac-208013-Pequena-pacote/dp/B01L9L0YP4/ref=zg_bs_electronics_28/132-5479222-0411803?pd_rd_i=B01L9L0YP4&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>#79</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Mi TV STICK Preto XIAOMI</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>R$ 279,99</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Xiaomi-Mi-TV-Stick/dp/B08GRM35BT/ref=zg_bs_electronics_29/132-5479222-0411803?pd_rd_i=B08GRM35BT&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>#80</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Tripé para bastão de selfie, 2 em 1 Suporte profissional multifuncional portátil para bastão de selfie de Bluetooth para telefone móvel Android/iOS, Suporte para tripé extensível leve Grampo para celu</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>R$ 37,89</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/profissional-multifuncional-port%C3%A1til-Bluetooth-extens%C3%ADvel/dp/B08C7249KP/ref=zg_bs_electronics_30/132-5479222-0411803?pd_rd_i=B08C7249KP&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>#81</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Celular Xiaomi Note 10S 8/128 Versão Global</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>R$ 1.656,09</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Celular-Xiaomi-Note-Vers%C3%A3o-Global/dp/B09B45YX56/ref=zg_bs_electronics_81/132-5479222-0411803?pd_rd_i=B09B45YX56&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>#82</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Galaxy Tab A7 Lite 4G 32GB 3G RAM Tela imersiva 8.7 pol - SM- T225</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>R$ 930,04</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Galaxy-Lite-Wi-Fi-32GB-imersiva/dp/B09B8HM8TT/ref=zg_bs_electronics_82/132-5479222-0411803?pd_rd_i=B09B8HM8TT&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>#83</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Novo Echo Show 8 (2ª Geração, versão 2021): Smart Display HD de 8" com Alexa e câmera de 13 MP - Cor Preta</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>R$ 999,00</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Echo-Show-8-segunda-gera%C3%A7%C3%A3o/dp/B084TNNRND/ref=zg_bs_electronics_83/132-5479222-0411803?pd_rd_i=B084TNNRND&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>#84</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Adaptador de Ethernet da Amazon para Fire TV</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>R$ 119,00</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Adaptador-Ethernet/dp/B086WCG4SR/ref=zg_bs_electronics_84/132-5479222-0411803?pd_rd_i=B086WCG4SR&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>#85</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Xiaomi Smartphone Redmi 9A 32GB 2GB RAM Dual Chip - Cinza</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>R$ 713,97</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-Redmi-Vers%C3%A3o-Global/dp/B08CGXVPXW/ref=zg_bs_electronics_85/132-5479222-0411803?pd_rd_i=B08CGXVPXW&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>#86</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Smartphone Samsung Galaxy A03 Core 32GB - Preto, 4G, Câmera 8MP + Selfie 5MP, Octa-Core, RAM 2GB, Tela 6,5"</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>R$ --------</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Samsung-Galaxy-Core-32GB/dp/B09QWWRB9L/ref=zg_bs_electronics_86/132-5479222-0411803?pd_rd_i=B09QWWRB9L&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>#87</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Kit Pilhas Alcalinas com 2X AA, Elgin, Baterias</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>R$ 4,95</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Kit-Pilhas-Alcalinas-Elgin-Baterias/dp/B0754JFB33/ref=zg_bs_electronics_87/132-5479222-0411803?pd_rd_i=B0754JFB33&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>#88</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Apple iPhone 12 (64 GB) - Preto</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>R$ 4.464,05</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Apple-iPhone-12-64-GB-Preto/dp/B09BG1CZ68/ref=zg_bs_electronics_88/132-5479222-0411803?pd_rd_i=B09BG1CZ68&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>#89</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Pilha, Rayovac, Alcalina 20324, Azul, AAA, Palito, Pacote de 4</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>R$ 11,63</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Pilha-Rayovac-20324-Palito-pacote/dp/B01L9L0ZRG/ref=zg_bs_electronics_89/132-5479222-0411803?pd_rd_i=B01L9L0ZRG&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>#90</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Smartphone Xiaomi Redmi Note 10s 64gb/6gb Ocean Blue</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>R$ 1.360,00</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-Redmi-Note-Ocean/dp/B097RF84GY/ref=zg_bs_electronics_90/132-5479222-0411803?pd_rd_i=B097RF84GY&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>#91</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Pilha Recarregável AAA Palito DURACELL Com 4 Unidades</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>R$ 99,52</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Pilha-Duracell-Recarreg%C3%A1vel-Aaa-unidades/dp/B000XSG300/ref=zg_bs_electronics_91/132-5479222-0411803?pd_rd_i=B000XSG300&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>#92</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Smartphone Xiaomi Poco M3 Pro 5g 6GB 128gb Global Power Black - Preto</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>R$ 1.432,17</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-128gb-Global-Power/dp/B097CLJMLD/ref=zg_bs_electronics_92/132-5479222-0411803?pd_rd_i=B097CLJMLD&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>#93</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Câmera de Segurança Doméstica Wi-Fi,  Tapo C100,  TP-Link</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>R$ 201,50</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/C%C3%A2mera-Seguran%C3%A7a-Dom%C3%A9stica-Wi-Fi-TP-Link/dp/B083V41T6M/ref=zg_bs_electronics_93/132-5479222-0411803?pd_rd_i=B083V41T6M&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>#94</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Smartphone Poco X3 PRO 256gb 8gb RAM - Metal Bronze - Dourado</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>R$ 2.203,99</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Poco-X3-PRO-256gb/dp/B0919LWHVK/ref=zg_bs_electronics_94/132-5479222-0411803?pd_rd_i=B0919LWHVK&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>#95</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Carregador De Pilhas Bivolt Para 4 Pilhas AA /AAA/ 9V + 2 Pilhas AA 1500mAh Ni-MH</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>R$ 86,07</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Carregador-Pilhas-Baterias-46RSCUSB0000-Elgin/dp/B07KX5W65P/ref=zg_bs_electronics_95/132-5479222-0411803?pd_rd_i=B07KX5W65P&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>#96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Celular Nokia 110 Preto com Rádio FM e Leitor Integrado, Câmera VGA e 4 Jogos - NK006</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>R$ 153,90</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Celular-Nokia-Leitor-Integrado-C%C3%A2mera/dp/B08WCCW92B/ref=zg_bs_electronics_96/132-5479222-0411803?pd_rd_i=B08WCCW92B&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>#97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Pilha Bateria Alcalina A23 Cartela com 5 Unidades 12V, Elgin, Baterias</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>R$ 16,90</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Bateria-Alcalina-Unidades-Elgin-Baterias/dp/B0765ZGFC2/ref=zg_bs_electronics_97/132-5479222-0411803?pd_rd_i=B0765ZGFC2&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>#98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Adaptador Para Tomada Pino Multiplicador Bipolar Branco, Force Line, 0180100015</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>R$ 5,33</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Tomada-Multiplicador-Bipolar-Branco-Force/dp/B07KFLPDLL/ref=zg_bs_electronics_98/132-5479222-0411803?pd_rd_i=B0884B4MJC&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>#99</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Smartphone Xiaomi Poco X3 GT 5G 256gb 8gb Cloud White - Branco</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>R$ 2.079,00</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Smartphone-Xiaomi-Poco-X3-GT/dp/B09C6Q977P/ref=zg_bs_electronics_99/132-5479222-0411803?pd_rd_i=B09C6Q977P&amp;psc=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>#100</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Celular Xiaomi Redmi Note 10S 6/64GB Cinza Global</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>R$ 1.399,00</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>https://www.amazon.com.br/Celular-Xiaomi-Redmi-Cinza-Global/dp/B09676KSYL/ref=zg_bs_electronics_100/132-5479222-0411803?pd_rd_i=B09676KSYL&amp;psc=1</t>
         </is>
       </c>
     </row>

</xml_diff>